<commit_message>
task1 and taskk2 updated
</commit_message>
<xml_diff>
--- a/Scraping Feasibility analysis-1.xlsx
+++ b/Scraping Feasibility analysis-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SrimathiP\Desktop\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeswa\OneDrive\Desktop\JMAN\JMAN-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F4DB47-1B14-4EAB-BA9F-E9C9CE564B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B04A9F9-D582-4B1F-9D6D-5EE27E3C19B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9293A5F0-AEBF-4395-AEF7-AF70B9C24D95}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{9293A5F0-AEBF-4395-AEF7-AF70B9C24D95}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="140">
   <si>
     <t>Project Overview</t>
   </si>
@@ -390,9 +390,6 @@
     <t>2.5s</t>
   </si>
   <si>
-    <t>Javascript rendered webpage</t>
-  </si>
-  <si>
     <t>Dutch</t>
   </si>
   <si>
@@ -417,9 +414,6 @@
     <t>Cookies pop up, reCAPTCHA,cloudfare</t>
   </si>
   <si>
-    <t>Cookies pop up</t>
-  </si>
-  <si>
     <t>257s</t>
   </si>
   <si>
@@ -442,22 +436,45 @@
   </si>
   <si>
     <t>90s</t>
+  </si>
+  <si>
+    <t>Javascript rendered webpage, 2019 requests per 10 mins</t>
+  </si>
+  <si>
+    <t>205 requests per 10 mins</t>
+  </si>
+  <si>
+    <t>196 requests per 10 mins</t>
+  </si>
+  <si>
+    <t>222 requests per 10 mins</t>
+  </si>
+  <si>
+    <t>Javascript rendered webpage, 722 requests per 10 mins</t>
+  </si>
+  <si>
+    <t>1 hr</t>
+  </si>
+  <si>
+    <t>6-10 hrs</t>
+  </si>
+  <si>
+    <t>Javascript based rendering website</t>
+  </si>
+  <si>
+    <t>Cookies pop up, Javascript based rendering website</t>
+  </si>
+  <si>
+    <t>Priem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -641,13 +658,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="2"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -711,7 +721,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -811,17 +821,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1012,164 +1011,198 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="dotted">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1619,63 +1652,63 @@
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.109375" style="1" customWidth="1"/>
-    <col min="6" max="8" width="15.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.21875" style="1" customWidth="1"/>
-    <col min="11" max="15" width="15.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.08984375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="15.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.1796875" style="1" customWidth="1"/>
+    <col min="11" max="15" width="15.81640625" style="1" customWidth="1"/>
     <col min="16" max="16" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.77734375" style="1"/>
+    <col min="17" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-    </row>
-    <row r="3" spans="1:16" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+    </row>
+    <row r="3" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-    </row>
-    <row r="5" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+    </row>
+    <row r="5" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -1690,14 +1723,14 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-    </row>
-    <row r="6" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+    </row>
+    <row r="6" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
         <v>3</v>
@@ -1712,14 +1745,14 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-    </row>
-    <row r="7" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+    </row>
+    <row r="7" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
         <v>5</v>
@@ -1734,14 +1767,14 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-    </row>
-    <row r="8" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+    </row>
+    <row r="8" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
         <v>7</v>
@@ -1756,70 +1789,70 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-    </row>
-    <row r="9" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-    </row>
-    <row r="10" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+    </row>
+    <row r="9" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+    </row>
+    <row r="10" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-    </row>
-    <row r="11" spans="1:16" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-    </row>
-    <row r="12" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+    </row>
+    <row r="11" spans="1:16" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+    </row>
+    <row r="12" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="s">
         <v>10</v>
@@ -1834,14 +1867,14 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-    </row>
-    <row r="13" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+    </row>
+    <row r="13" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
         <v>11</v>
@@ -1854,14 +1887,14 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-    </row>
-    <row r="14" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+    </row>
+    <row r="14" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
         <v>12</v>
@@ -1874,70 +1907,70 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
-    </row>
-    <row r="15" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-    </row>
-    <row r="16" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+    </row>
+    <row r="15" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+    </row>
+    <row r="16" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
       <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-    </row>
-    <row r="17" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-    </row>
-    <row r="18" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+    </row>
+    <row r="17" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+    </row>
+    <row r="18" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="13" t="s">
         <v>14</v>
@@ -1952,14 +1985,14 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-    </row>
-    <row r="19" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+    </row>
+    <row r="19" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13" t="s">
         <v>16</v>
@@ -1972,14 +2005,14 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-    </row>
-    <row r="20" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+    </row>
+    <row r="20" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="13" t="s">
         <v>17</v>
@@ -1994,14 +2027,14 @@
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-    </row>
-    <row r="21" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+    </row>
+    <row r="21" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="13" t="s">
         <v>18</v>
@@ -2014,14 +2047,14 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-    </row>
-    <row r="22" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+    </row>
+    <row r="22" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
         <v>19</v>
@@ -2034,14 +2067,14 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-    </row>
-    <row r="23" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+    </row>
+    <row r="23" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>20</v>
@@ -2056,14 +2089,14 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-    </row>
-    <row r="24" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+    </row>
+    <row r="24" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
         <v>21</v>
@@ -2078,14 +2111,14 @@
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-    </row>
-    <row r="25" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+    </row>
+    <row r="25" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="13" t="s">
         <v>22</v>
@@ -2098,32 +2131,32 @@
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-    </row>
-    <row r="26" spans="1:16" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="34"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-    </row>
-    <row r="27" spans="1:16" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+    </row>
+    <row r="26" spans="1:16" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+    </row>
+    <row r="27" spans="1:16" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="17" t="s">
         <v>23</v>
@@ -2143,7 +2176,7 @@
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
     </row>
-    <row r="28" spans="1:16" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="19">
         <f>COUNT('Web Scraping Feasibility'!B8:B12)</f>
@@ -2151,11 +2184,11 @@
       </c>
       <c r="C28" s="19">
         <f>COUNTIF('Web Scraping Feasibility'!Q8:Q12, "Easy")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" s="19">
         <f>COUNTIF('Web Scraping Feasibility'!Q8:Q12, "Moderate")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="19">
         <f>COUNTIF('Web Scraping Feasibility'!Q8:Q12, "Hard")</f>
@@ -2166,155 +2199,155 @@
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="34"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="34"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="40" t="s">
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="32"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+    </row>
+    <row r="35" spans="2:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B35" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="34"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="34" t="s">
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="32"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="34"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="39"/>
+      <c r="E36" s="32"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="34"/>
-      <c r="C40" s="42" t="s">
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="32"/>
+      <c r="C40" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="42" t="s">
+      <c r="D40" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="34"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="34"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="34"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="34"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="34"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="34"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="34"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="34"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="34"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="32"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="32"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="32"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="32"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="32"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="32"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="32"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="32"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="32"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-    </row>
-    <row r="49" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B49" s="55" t="s">
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+    </row>
+    <row r="49" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B49" s="53" t="s">
         <v>80</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B50" s="55" t="s">
+    <row r="50" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" s="53" t="s">
         <v>81</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B51" s="55" t="s">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="53" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B52" s="55" t="s">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="53" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B53" s="43"/>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="41"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2329,60 +2362,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB2C782-2303-414A-B12B-FF8717ED39A2}">
-  <dimension ref="A2:V39"/>
+  <dimension ref="A2:V36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="I8" sqref="I8"/>
+      <selection pane="topRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="26.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="30.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.5546875" style="1" customWidth="1"/>
-    <col min="13" max="14" width="23.77734375" style="1" customWidth="1"/>
-    <col min="15" max="16" width="29.5546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="23.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="35.21875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="23.77734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="31.21875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="70.77734375" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.77734375" style="1"/>
+    <col min="9" max="9" width="22.08984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="40.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.54296875" style="1" customWidth="1"/>
+    <col min="13" max="14" width="23.81640625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="29.54296875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="23.81640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="35.1796875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.81640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="31.1796875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="70.81640625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
+    <row r="2" spans="1:22" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
     </row>
     <row r="3" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
@@ -2408,7 +2442,7 @@
       <c r="S3" s="21"/>
       <c r="T3" s="21"/>
       <c r="U3" s="21"/>
-      <c r="V3" s="34"/>
+      <c r="V3" s="32"/>
     </row>
     <row r="4" spans="1:22" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
@@ -2432,38 +2466,38 @@
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
       <c r="U4" s="25"/>
-      <c r="V4" s="44"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
+      <c r="V4" s="42"/>
+    </row>
+    <row r="5" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
       <c r="B5" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+    </row>
+    <row r="7" spans="1:22" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
       <c r="B7" s="17" t="s">
         <v>38</v>
       </c>
@@ -2524,17 +2558,17 @@
       <c r="U7" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="V7" s="34"/>
-    </row>
-    <row r="8" spans="1:22" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="47">
+      <c r="V7" s="32"/>
+    </row>
+    <row r="8" spans="1:22" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="45">
         <v>1</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="50" t="s">
         <v>106</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -2544,18 +2578,20 @@
         <v>56</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="53"/>
+        <v>57</v>
+      </c>
+      <c r="K8" s="51" t="s">
+        <v>137</v>
+      </c>
       <c r="L8" s="28" t="s">
         <v>58</v>
       </c>
@@ -2565,9 +2601,11 @@
       <c r="N8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="O8" s="3"/>
+      <c r="O8" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="P8" s="3" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>60</v>
@@ -2578,21 +2616,21 @@
       <c r="S8" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="T8" s="51"/>
+      <c r="T8" s="49"/>
       <c r="U8" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="V8" s="34"/>
-    </row>
-    <row r="9" spans="1:22" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="48">
+        <v>134</v>
+      </c>
+      <c r="V8" s="32"/>
+    </row>
+    <row r="9" spans="1:22" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="46">
         <v>2</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="D9" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>107</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -2608,15 +2646,15 @@
         <v>113</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="L9" s="28" t="s">
+      <c r="K9" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="L9" s="75" t="s">
         <v>58</v>
       </c>
       <c r="M9" s="3" t="s">
@@ -2625,9 +2663,11 @@
       <c r="N9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="O9" s="3"/>
+      <c r="O9" s="31" t="s">
+        <v>136</v>
+      </c>
       <c r="P9" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>26</v>
@@ -2638,22 +2678,24 @@
       <c r="S9" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="T9" s="54" t="s">
+      <c r="T9" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="U9" s="10"/>
-      <c r="V9" s="34"/>
-    </row>
-    <row r="10" spans="1:22" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="48">
+      <c r="U9" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="V9" s="32"/>
+    </row>
+    <row r="10" spans="1:22" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="46">
         <v>3</v>
       </c>
-      <c r="C10" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>128</v>
+      <c r="C10" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>126</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>101</v>
@@ -2668,13 +2710,13 @@
         <v>111</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>57</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L10" s="28" t="s">
         <v>58</v>
@@ -2682,12 +2724,14 @@
       <c r="M10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3" t="s">
-        <v>115</v>
+      <c r="O10" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>114</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>26</v>
@@ -2698,21 +2742,23 @@
       <c r="S10" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="T10" s="54" t="s">
+      <c r="T10" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="U10" s="10"/>
-      <c r="V10" s="34"/>
-    </row>
-    <row r="11" spans="1:22" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="48">
+      <c r="U10" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="V10" s="32"/>
+    </row>
+    <row r="11" spans="1:22" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="46">
         <v>4</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="50" t="s">
         <v>108</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -2722,7 +2768,7 @@
         <v>56</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>76</v>
@@ -2734,7 +2780,7 @@
         <v>57</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="L11" s="28" t="s">
         <v>58</v>
@@ -2745,12 +2791,14 @@
       <c r="N11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="O11" s="3"/>
+      <c r="O11" s="72" t="s">
+        <v>135</v>
+      </c>
       <c r="P11" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="R11" s="3" t="s">
         <v>59</v>
@@ -2760,54 +2808,56 @@
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="V11" s="34"/>
-    </row>
-    <row r="12" spans="1:22" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="49">
+        <v>130</v>
+      </c>
+      <c r="V11" s="32"/>
+    </row>
+    <row r="12" spans="1:22" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="47">
         <v>5</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="62" t="s">
-        <v>127</v>
+        <v>119</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>125</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="74" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="75" t="s">
         <v>76</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="J12" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J12" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="L12" s="32" t="s">
+      <c r="K12" s="75" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="33" t="s">
+      <c r="M12" s="75" t="s">
         <v>58</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="O12" s="3"/>
+      <c r="O12" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="P12" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>60</v>
@@ -2821,478 +2871,472 @@
       <c r="T12" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="U12" s="10"/>
-      <c r="V12" s="34"/>
-    </row>
-    <row r="17" spans="3:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="52"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-    </row>
-    <row r="18" spans="3:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="64"/>
-    </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="34"/>
-      <c r="U19" s="34"/>
-      <c r="V19" s="34"/>
-    </row>
-    <row r="20" spans="3:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="C20" s="34"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="34"/>
-    </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="34"/>
-    </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="34"/>
-    </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="34"/>
-    </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="34"/>
-      <c r="V24" s="34"/>
-    </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="34"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="34"/>
-    </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="34"/>
-    </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="34"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="34"/>
-      <c r="V27" s="34"/>
-    </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="34"/>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="34"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="34"/>
-      <c r="S29" s="34"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="34"/>
-      <c r="V29" s="34"/>
-    </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
-      <c r="S30" s="34"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="34"/>
-      <c r="V30" s="34"/>
-    </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
-      <c r="O31" s="34"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="34"/>
-      <c r="R31" s="34"/>
-      <c r="S31" s="34"/>
-      <c r="T31" s="34"/>
-      <c r="U31" s="34"/>
-      <c r="V31" s="34"/>
-    </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="34"/>
-      <c r="T32" s="34"/>
-      <c r="U32" s="34"/>
-      <c r="V32" s="34"/>
-    </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="34"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="34"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
-      <c r="V33" s="34"/>
-    </row>
-    <row r="34" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="34"/>
-      <c r="P34" s="34"/>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="34"/>
-      <c r="T34" s="34"/>
-      <c r="U34" s="34"/>
-      <c r="V34" s="34"/>
-    </row>
-    <row r="35" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="34"/>
-      <c r="P35" s="34"/>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="34"/>
-      <c r="S35" s="34"/>
-      <c r="T35" s="34"/>
-      <c r="U35" s="34"/>
-      <c r="V35" s="34"/>
-    </row>
-    <row r="36" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="34"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="34"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="34"/>
-    </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="34"/>
-      <c r="P37" s="34"/>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="34"/>
-      <c r="S37" s="34"/>
-      <c r="T37" s="34"/>
-      <c r="U37" s="34"/>
-      <c r="V37" s="34"/>
-    </row>
-    <row r="38" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="34"/>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="34"/>
-      <c r="S38" s="34"/>
-      <c r="T38" s="34"/>
-      <c r="U38" s="34"/>
-      <c r="V38" s="34"/>
-    </row>
-    <row r="39" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="34"/>
-      <c r="U39" s="34"/>
-      <c r="V39" s="34"/>
+      <c r="U12" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="V12" s="32"/>
+    </row>
+    <row r="16" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+    </row>
+    <row r="17" spans="3:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="C17" s="32"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+    </row>
+    <row r="18" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+    </row>
+    <row r="19" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+    </row>
+    <row r="20" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+    </row>
+    <row r="21" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+    </row>
+    <row r="22" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+    </row>
+    <row r="23" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="32"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+    </row>
+    <row r="24" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="32"/>
+      <c r="U24" s="32"/>
+      <c r="V24" s="32"/>
+    </row>
+    <row r="25" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+    </row>
+    <row r="26" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="32"/>
+      <c r="V26" s="32"/>
+    </row>
+    <row r="27" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="32"/>
+      <c r="V27" s="32"/>
+    </row>
+    <row r="28" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="32"/>
+      <c r="U28" s="32"/>
+      <c r="V28" s="32"/>
+    </row>
+    <row r="29" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="32"/>
+    </row>
+    <row r="30" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="32"/>
+    </row>
+    <row r="31" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+    </row>
+    <row r="32" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
+    </row>
+    <row r="33" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+    </row>
+    <row r="34" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="32"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="32"/>
+    </row>
+    <row r="35" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="32"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="32"/>
+      <c r="V35" s="32"/>
+    </row>
+    <row r="36" spans="3:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q8:Q12">
@@ -3351,700 +3395,700 @@
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="38.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.21875" style="1" customWidth="1"/>
-    <col min="10" max="14" width="15.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="38.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" style="1" customWidth="1"/>
+    <col min="10" max="14" width="15.81640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.77734375" style="1"/>
+    <col min="16" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-    </row>
-    <row r="3" spans="2:15" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+    </row>
+    <row r="3" spans="2:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-    </row>
-    <row r="4" spans="2:15" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+    </row>
+    <row r="4" spans="2:15" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+    </row>
+    <row r="5" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-    </row>
-    <row r="7" spans="2:15" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="39" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+    </row>
+    <row r="7" spans="2:15" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-    </row>
-    <row r="8" spans="2:15" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="68">
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+    </row>
+    <row r="8" spans="2:15" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="64">
         <v>1</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-    </row>
-    <row r="9" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="69"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="56" t="s">
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+    </row>
+    <row r="9" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="65"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-    </row>
-    <row r="10" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="69"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="56" t="s">
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+    </row>
+    <row r="10" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="65"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-    </row>
-    <row r="11" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="69"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="56" t="s">
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+    </row>
+    <row r="11" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="65"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-    </row>
-    <row r="12" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="69"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="56" t="s">
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+    </row>
+    <row r="12" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="65"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-    </row>
-    <row r="13" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="69"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="56" t="s">
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+    </row>
+    <row r="13" spans="2:15" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="65"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-    </row>
-    <row r="14" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="69"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="38" t="s">
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="65"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-    </row>
-    <row r="15" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="69"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="56" t="s">
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+    </row>
+    <row r="15" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="65"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-    </row>
-    <row r="16" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="70"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="58" t="s">
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+    </row>
+    <row r="16" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="66"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-    </row>
-    <row r="17" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="71">
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+    </row>
+    <row r="17" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="67">
         <v>2</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-    </row>
-    <row r="18" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="69"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="59" t="s">
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="65"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-    </row>
-    <row r="19" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="69"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="37" t="s">
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+    </row>
+    <row r="19" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="65"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-    </row>
-    <row r="20" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="69"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="38" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+    </row>
+    <row r="20" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="65"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-    </row>
-    <row r="21" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="69"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="38" t="s">
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+    </row>
+    <row r="21" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" s="65"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-    </row>
-    <row r="22" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="69"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="38" t="s">
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+    </row>
+    <row r="22" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="65"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-    </row>
-    <row r="23" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B23" s="69"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="56" t="s">
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+    </row>
+    <row r="23" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" s="65"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-    </row>
-    <row r="24" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B24" s="70"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="57" t="s">
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+    </row>
+    <row r="24" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B24" s="66"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-    </row>
-    <row r="25" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B25" s="71">
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+    </row>
+    <row r="25" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="67">
         <v>3</v>
       </c>
-      <c r="C25" s="72" t="s">
+      <c r="C25" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-    </row>
-    <row r="26" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B26" s="69"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="59" t="s">
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+    </row>
+    <row r="26" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="65"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-    </row>
-    <row r="27" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B27" s="69"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="37" t="s">
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+    </row>
+    <row r="27" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="65"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-    </row>
-    <row r="28" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B28" s="69"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="37" t="s">
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+    </row>
+    <row r="28" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="65"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-    </row>
-    <row r="29" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B29" s="69"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="56" t="s">
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+    </row>
+    <row r="29" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29" s="65"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-    </row>
-    <row r="30" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B30" s="69"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="38" t="s">
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+    </row>
+    <row r="30" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="65"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B31" s="69"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="38" t="s">
+    <row r="31" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B31" s="65"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B32" s="69"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="38" t="s">
+    <row r="32" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B32" s="65"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B33" s="69"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="56" t="s">
+    <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B33" s="65"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="54" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B34" s="70"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="57" t="s">
+    <row r="34" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B34" s="66"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="55" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B35" s="71">
+    <row r="35" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="67">
         <v>4</v>
       </c>
-      <c r="C35" s="73" t="s">
+      <c r="C35" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B36" s="69"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="59" t="s">
+    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36" s="65"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="57" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B37" s="69"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="37" t="s">
+    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B37" s="65"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B38" s="69"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="37" t="s">
+    <row r="38" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B38" s="65"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B39" s="69"/>
-      <c r="C39" s="74"/>
-      <c r="D39" s="56" t="s">
+    <row r="39" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="65"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="54" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B40" s="69"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="38" t="s">
+    <row r="40" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" s="65"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B41" s="69"/>
-      <c r="C41" s="74"/>
-      <c r="D41" s="38" t="s">
+    <row r="41" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B41" s="65"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B42" s="69"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="56" t="s">
+    <row r="42" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B42" s="65"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="54" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B43" s="70"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="57" t="s">
+    <row r="43" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B43" s="66"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="55" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B44" s="71">
+    <row r="44" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" s="67">
         <v>5</v>
       </c>
-      <c r="C44" s="72" t="s">
+      <c r="C44" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="D44" s="34" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B45" s="69"/>
-      <c r="C45" s="66"/>
-      <c r="D45" s="56" t="s">
+    <row r="45" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="65"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="54" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B46" s="69"/>
-      <c r="C46" s="66"/>
-      <c r="D46" s="59" t="s">
+    <row r="46" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="65"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="57" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B47" s="69"/>
-      <c r="C47" s="66"/>
-      <c r="D47" s="38" t="s">
+    <row r="47" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" s="65"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="36" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B48" s="69"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="56" t="s">
+    <row r="48" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B48" s="65"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="54" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B49" s="69"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="56" t="s">
+    <row r="49" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B49" s="65"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="54" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B50" s="69"/>
-      <c r="C50" s="66"/>
-      <c r="D50" s="38" t="s">
+    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" s="65"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B51" s="70"/>
-      <c r="C51" s="67"/>
-      <c r="D51" s="57" t="s">
+    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B51" s="66"/>
+      <c r="C51" s="63"/>
+      <c r="D51" s="55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B52" s="71">
+    <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B52" s="67">
         <v>6</v>
       </c>
-      <c r="C52" s="72" t="s">
+      <c r="C52" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="37" t="s">
+      <c r="D52" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B53" s="69"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="56" t="s">
+    <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B53" s="65"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="54" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B54" s="69"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="38" t="s">
+    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B54" s="65"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="36" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B55" s="69"/>
-      <c r="C55" s="66"/>
-      <c r="D55" s="38" t="s">
+    <row r="55" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" s="65"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="36" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B56" s="69"/>
-      <c r="C56" s="66"/>
-      <c r="D56" s="56" t="s">
+    <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B56" s="65"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="54" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B57" s="69"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="37" t="s">
+    <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B57" s="65"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B58" s="69"/>
-      <c r="C58" s="66"/>
-      <c r="D58" s="59" t="s">
+    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B58" s="65"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="57" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B59" s="69"/>
-      <c r="C59" s="66"/>
-      <c r="D59" s="37" t="s">
+    <row r="59" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B59" s="65"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B60" s="69"/>
-      <c r="C60" s="66"/>
-      <c r="D60" s="38" t="s">
+    <row r="60" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B60" s="65"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B61" s="69"/>
-      <c r="C61" s="66"/>
-      <c r="D61" s="38" t="s">
+    <row r="61" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B61" s="65"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B62" s="69"/>
-      <c r="C62" s="66"/>
-      <c r="D62" s="56" t="s">
+    <row r="62" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B62" s="65"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="54" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B63" s="70"/>
-      <c r="C63" s="67"/>
-      <c r="D63" s="57" t="s">
+    <row r="63" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B63" s="66"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="55" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4077,9 +4121,9 @@
       <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -4087,7 +4131,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -4095,7 +4139,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -4103,7 +4147,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -4114,30 +4158,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ec677dc8-5d48-4172-a0f7-8caa86e594ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="018ae51e-e50b-4164-b6ec-f6a1266956f6"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<SyracuseOfficeCustomData>{"createMode":"plain_doc","forceRefresh":"0"}</SyracuseOfficeCustomData>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060DD271887131D4BABC2898D91048802" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="054418bf43d6985c6bb4236577442967">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ec677dc8-5d48-4172-a0f7-8caa86e594ca" xmlns:ns3="018ae51e-e50b-4164-b6ec-f6a1266956f6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae30e0dd79b20a58e0494251b1c40fac" ns2:_="" ns3:_="">
     <xsd:import namespace="ec677dc8-5d48-4172-a0f7-8caa86e594ca"/>
@@ -4392,38 +4412,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F63D4D81-219B-4355-BF20-0227D685F5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="018ae51e-e50b-4164-b6ec-f6a1266956f6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ec677dc8-5d48-4172-a0f7-8caa86e594ca"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<SyracuseOfficeCustomData>{"createMode":"plain_doc","forceRefresh":"0"}</SyracuseOfficeCustomData>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{231AE957-FDC7-45B5-BE48-153BD871AC5F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48CC9458-8240-4EFE-9A82-B325EE52E81E}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ec677dc8-5d48-4172-a0f7-8caa86e594ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="018ae51e-e50b-4164-b6ec-f6a1266956f6"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BEB30D3-16D6-49D3-9CF2-6E798F1B5F95}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4440,4 +4453,35 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48CC9458-8240-4EFE-9A82-B325EE52E81E}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{231AE957-FDC7-45B5-BE48-153BD871AC5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F63D4D81-219B-4355-BF20-0227D685F5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="018ae51e-e50b-4164-b6ec-f6a1266956f6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ec677dc8-5d48-4172-a0f7-8caa86e594ca"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>